<commit_message>
campi da riempire gialli
</commit_message>
<xml_diff>
--- a/FogliCalcolo/AntiIncendio/AntiIncendio.xlsx
+++ b/FogliCalcolo/AntiIncendio/AntiIncendio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giona\Desktop\git\ImpiantiMeccanici\FogliCalcolo\AntiIncendio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC81D753-5605-4AB9-B1DE-46FD2DB70841}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F6F2BA-03A6-4151-9485-7BB042553A95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{814501E0-9C7E-4A9C-BA68-550DD9DF6520}"/>
   </bookViews>
@@ -543,12 +543,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -680,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -699,9 +705,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -711,7 +714,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -721,15 +723,49 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -748,40 +784,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1113,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{942DB0D8-C548-4966-8C5B-96C53EE50420}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,29 +1151,29 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="2"/>
-      <c r="P2" s="26" t="s">
+      <c r="P2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="Q2" s="28"/>
+      <c r="Q2" s="36"/>
     </row>
     <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="45">
         <v>60</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -1171,7 +1183,7 @@
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="45">
         <v>2.75</v>
       </c>
       <c r="H3" s="10" t="s">
@@ -1190,17 +1202,17 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="45">
         <v>30</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="45">
         <v>50</v>
       </c>
       <c r="H4" s="10" t="s">
@@ -1223,11 +1235,11 @@
         <f>C3/C4</f>
         <v>2</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="35"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="12">
         <f>G4*0.0689475729</f>
         <v>3.4473786450000001</v>
@@ -1239,7 +1251,7 @@
       <c r="P5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="Q5" s="17" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1259,7 +1271,7 @@
       <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="46">
         <v>80</v>
       </c>
       <c r="H6" s="11" t="s">
@@ -1275,10 +1287,10 @@
     </row>
     <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="45">
         <v>0.5</v>
       </c>
       <c r="D7" s="10"/>
@@ -1290,16 +1302,16 @@
       <c r="P7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="Q7" s="17" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="45">
         <v>7</v>
       </c>
       <c r="D8" s="10"/>
@@ -1311,7 +1323,7 @@
       <c r="P8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Q8" s="19" t="s">
+      <c r="Q8" s="17" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1324,7 +1336,7 @@
         <f>PI()*G3^2</f>
         <v>23.758294442772812</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="2"/>
@@ -1332,10 +1344,10 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="P9" s="20" t="s">
+      <c r="P9" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="Q9" s="19" t="s">
+      <c r="Q9" s="17" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1354,10 +1366,10 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="P10" s="20" t="s">
+      <c r="P10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="Q10" s="19" t="s">
+      <c r="Q10" s="17" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1365,7 +1377,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="P11" s="20" t="s">
+      <c r="P11" s="18" t="s">
         <v>47</v>
       </c>
       <c r="Q11" s="10" t="s">
@@ -1373,44 +1385,44 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="29" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="13"/>
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="31"/>
-      <c r="L12" s="32" t="s">
+      <c r="I12" s="40"/>
+      <c r="J12" s="41"/>
+      <c r="L12" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="M12" s="33"/>
-      <c r="N12" s="34"/>
-      <c r="P12" s="40" t="s">
+      <c r="M12" s="43"/>
+      <c r="N12" s="44"/>
+      <c r="P12" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="41" t="s">
+      <c r="Q12" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="1">
+      <c r="B13" s="47">
         <v>3</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="45">
         <f>_xlfn.CEILING.MATH(B13/$C$5)</f>
         <v>2</v>
       </c>
@@ -1430,7 +1442,7 @@
       <c r="H13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="19">
         <f>G5^0.5*G6</f>
         <v>148.53694263717696</v>
       </c>
@@ -1440,7 +1452,7 @@
       <c r="L13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="45">
         <v>60</v>
       </c>
       <c r="N13" s="10" t="s">
@@ -1454,11 +1466,11 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="B14" s="1">
+      <c r="B14" s="47">
         <f>B13+1</f>
         <v>4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="45">
         <f t="shared" ref="C14:C40" si="0">_xlfn.CEILING.MATH(B14/$C$5)</f>
         <v>2</v>
       </c>
@@ -1475,10 +1487,10 @@
         <v>0.10559241974565695</v>
       </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="19">
         <f>I13*D40*C7</f>
         <v>6758.4308899915522</v>
       </c>
@@ -1488,7 +1500,7 @@
       <c r="L14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="45">
         <v>1.2</v>
       </c>
       <c r="N14" s="10"/>
@@ -1500,11 +1512,11 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="1">
+      <c r="B15" s="47">
         <f t="shared" ref="B15:B39" si="4">B14+1</f>
         <v>5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="45">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1520,8 +1532,8 @@
         <f t="shared" si="3"/>
         <v>0.19798578702310676</v>
       </c>
-      <c r="H15" s="35"/>
-      <c r="I15" s="25">
+      <c r="H15" s="37"/>
+      <c r="I15" s="23">
         <f>I14*0.001/60</f>
         <v>0.11264051483319254</v>
       </c>
@@ -1546,11 +1558,11 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
+      <c r="B16" s="47">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="45">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1569,7 +1581,7 @@
       <c r="H16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="45">
         <v>3</v>
       </c>
       <c r="J16" s="10" t="s">
@@ -1583,11 +1595,11 @@
       </c>
     </row>
     <row r="17" spans="2:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="B17" s="1">
+      <c r="B17" s="47">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="45">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1606,14 +1618,14 @@
       <c r="H17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="23">
         <f>(4*I15/(PI()*I16))^0.5</f>
         <v>0.21864610509904539</v>
       </c>
       <c r="J17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P17" s="20" t="s">
+      <c r="P17" s="18" t="s">
         <v>46</v>
       </c>
       <c r="Q17" s="10" t="s">
@@ -1621,11 +1633,11 @@
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
+      <c r="B18" s="47">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="45">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1644,7 +1656,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="2"/>
       <c r="J18" s="10"/>
-      <c r="P18" s="23" t="s">
+      <c r="P18" s="21" t="s">
         <v>68</v>
       </c>
       <c r="Q18" s="10" t="s">
@@ -1652,11 +1664,11 @@
       </c>
     </row>
     <row r="19" spans="2:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="B19" s="1">
+      <c r="B19" s="47">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="45">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1675,23 +1687,23 @@
       <c r="H19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="45">
         <v>0.21909999999999999</v>
       </c>
       <c r="J19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P19" s="36" t="s">
+      <c r="P19" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="Q19" s="37"/>
+      <c r="Q19" s="32"/>
     </row>
     <row r="20" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="1">
+      <c r="B20" s="47">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="45">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1710,21 +1722,21 @@
       <c r="H20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="45">
         <v>2.3E-3</v>
       </c>
       <c r="J20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="39"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="34"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
+      <c r="B21" s="47">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="45">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1752,11 +1764,11 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
+      <c r="B22" s="47">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="45">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1777,11 +1789,11 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="1">
+      <c r="B23" s="47">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="45">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1800,20 +1812,20 @@
       <c r="H23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="45">
         <v>12</v>
       </c>
       <c r="J23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="R23" s="22"/>
+      <c r="R23" s="20"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="1">
+      <c r="B24" s="47">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="45">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1832,20 +1844,20 @@
       <c r="H24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="45">
         <v>200</v>
       </c>
       <c r="J24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R24" s="22"/>
+      <c r="R24" s="20"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="1">
+      <c r="B25" s="47">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="45">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1864,22 +1876,22 @@
       <c r="H25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="45">
         <v>20</v>
       </c>
       <c r="J25" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="22"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
     </row>
     <row r="26" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="1">
+      <c r="B26" s="47">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="45">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1907,11 +1919,11 @@
       </c>
     </row>
     <row r="27" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="1">
+      <c r="B27" s="47">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="45">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1929,11 +1941,11 @@
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="1">
+      <c r="B28" s="47">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="45">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1949,18 +1961,18 @@
         <f t="shared" si="3"/>
         <v>2.138246499849553</v>
       </c>
-      <c r="H28" s="26" t="s">
+      <c r="H28" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="I28" s="27"/>
-      <c r="J28" s="28"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="1">
+      <c r="B29" s="47">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="45">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1988,11 +2000,11 @@
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B30" s="1">
+      <c r="B30" s="47">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="45">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -2011,17 +2023,17 @@
       <c r="H30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="45">
         <v>0.95</v>
       </c>
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="1">
+      <c r="B31" s="47">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="45">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2040,17 +2052,17 @@
       <c r="H31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="45">
         <v>0.85</v>
       </c>
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="1">
+      <c r="B32" s="47">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="45">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2069,17 +2081,17 @@
       <c r="H32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="45">
         <v>0.9</v>
       </c>
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="1">
+      <c r="B33" s="47">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="45">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2107,11 +2119,11 @@
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="1">
+      <c r="B34" s="47">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="45">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2132,11 +2144,11 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="1">
+      <c r="B35" s="47">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="45">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2155,7 +2167,7 @@
       <c r="H35" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="45">
         <v>4</v>
       </c>
       <c r="J35" s="10" t="s">
@@ -2163,11 +2175,11 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B36" s="1">
+      <c r="B36" s="47">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="45">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2186,7 +2198,7 @@
       <c r="H36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="45">
         <v>0.15</v>
       </c>
       <c r="J36" s="10" t="s">
@@ -2194,11 +2206,11 @@
       </c>
     </row>
     <row r="37" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B37" s="1">
+      <c r="B37" s="47">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="45">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2217,7 +2229,7 @@
       <c r="H37" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="45">
         <v>2</v>
       </c>
       <c r="J37" s="10" t="s">
@@ -2225,11 +2237,11 @@
       </c>
     </row>
     <row r="38" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="1">
+      <c r="B38" s="47">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="45">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2257,11 +2269,11 @@
       </c>
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="5">
+      <c r="B39" s="48">
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="46">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -2279,22 +2291,22 @@
       </c>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="14">
+      <c r="B40" s="49">
         <v>13</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="50">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="14">
         <f t="shared" ref="D40" si="5">B40*C40</f>
         <v>91</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E40" s="15">
         <f t="shared" si="2"/>
         <v>2162.0047942923256</v>
       </c>
-      <c r="F40" s="17">
+      <c r="F40" s="16">
         <f t="shared" si="3"/>
         <v>1.2011137746068477</v>
       </c>
@@ -2307,6 +2319,8 @@
     <sortCondition ref="P3:P18"/>
   </sortState>
   <mergeCells count="9">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="H14:H15"/>
     <mergeCell ref="P19:Q20"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="F4:F5"/>
@@ -2314,8 +2328,6 @@
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="L12:N12"/>
     <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <conditionalFormatting sqref="D13:D39">
     <cfRule type="expression" priority="8">

</xml_diff>